<commit_message>
some enhancements to add notebook capability
</commit_message>
<xml_diff>
--- a/docs/find_dupicates-layout.xlsx
+++ b/docs/find_dupicates-layout.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Enhancements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Select Folders</t>
   </si>
@@ -61,13 +62,73 @@
   </si>
   <si>
     <t>mainsizer</t>
+  </si>
+  <si>
+    <t>Clear Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Find Duplicates</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compare Folders</t>
+  </si>
+  <si>
+    <t>Folder 1</t>
+  </si>
+  <si>
+    <t>Folder 2</t>
+  </si>
+  <si>
+    <t>Folders to Exclude</t>
+  </si>
+  <si>
+    <t>Skip Matches</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> o  Compare Folders</t>
+  </si>
+  <si>
+    <t>o  Find Duplicates</t>
+  </si>
+  <si>
+    <t>(Power Options)</t>
+  </si>
+  <si>
+    <t>Compare View</t>
+  </si>
+  <si>
+    <t>Standard View</t>
+  </si>
+  <si>
+    <t>Delete Selected</t>
+  </si>
+  <si>
+    <t>Right click for more options</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>Select Exclusions</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>+ Size x 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,8 +181,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,8 +228,26 @@
     <fill>
       <patternFill patternType="lightHorizontal"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -544,8 +630,362 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -562,8 +1002,56 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,99 +1065,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -681,29 +1085,353 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="56" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="58" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="43" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="64">
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
@@ -1038,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:O26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1083,26 +1811,26 @@
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="50"/>
+      <c r="E3" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="50"/>
+      <c r="G3" s="4"/>
+      <c r="J3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="20" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="4"/>
-      <c r="J3" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="35">
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="10">
         <v>1</v>
       </c>
     </row>
@@ -1110,31 +1838,31 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="34">
+      <c r="P4" s="21">
         <v>2</v>
       </c>
     </row>
@@ -1142,514 +1870,518 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="22" t="s">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="47" t="s">
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="34"/>
+      <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
-      <c r="J6" s="40" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="J6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="34"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="21"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="6"/>
-      <c r="J7" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="34"/>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="J7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="34"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="1:16" ht="16" thickBot="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="J8" s="41" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="J8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="J9" s="25" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="J9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="35">
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="35">
+      <c r="B10" s="34"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="35"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="35"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="35"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="35"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="35"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="6"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="35"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="2"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="6"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="35"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="35"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="2"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="6"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="35"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="2"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="6"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="35"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="2"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="35"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="10"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="2"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="6"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="35"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="10"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="2"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="35"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="10"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="2"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="6"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="35"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="31"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="10"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="2"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="35"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="10"/>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="2"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="10"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="2">
         <v>8</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-      <c r="J27" s="11" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="J27" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="35">
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="2"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="6"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="35">
+      <c r="B28" s="34"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="31"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="2"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="6"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="35"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="10"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="2"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="6"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="35"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="31"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="10"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="2"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="35"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="33"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:16" ht="16" thickBot="1">
       <c r="A32" s="2">
         <v>9</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="10"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="35">
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="20"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="10">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="K6:O8"/>
+    <mergeCell ref="J10:O26"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J28:O31"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="J3:L3"/>
     <mergeCell ref="J32:O32"/>
     <mergeCell ref="P4:P8"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="J9:O9"/>
     <mergeCell ref="C6:G8"/>
@@ -1660,10 +2392,866 @@
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="K6:O8"/>
-    <mergeCell ref="J10:O26"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J28:O31"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:V38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" ht="16" thickBot="1">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22">
+      <c r="C3" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="82"/>
+      <c r="H3" s="83"/>
+      <c r="J3" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="105" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="112" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="114"/>
+      <c r="Q4" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="112" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="114"/>
+    </row>
+    <row r="5" spans="2:22">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="106"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="115"/>
+      <c r="Q5" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="106"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="115"/>
+    </row>
+    <row r="6" spans="2:22" ht="16" thickBot="1">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+      <c r="J6" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="116"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="118"/>
+      <c r="Q6" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="116"/>
+      <c r="S6" s="117"/>
+      <c r="T6" s="117"/>
+      <c r="U6" s="117"/>
+      <c r="V6" s="118"/>
+    </row>
+    <row r="7" spans="2:22">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+      <c r="J7" s="108" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="109"/>
+      <c r="Q7" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" s="99"/>
+      <c r="S7" s="99"/>
+      <c r="T7" s="99"/>
+      <c r="U7" s="99"/>
+      <c r="V7" s="100"/>
+    </row>
+    <row r="8" spans="2:22">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="J8" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="91"/>
+      <c r="Q8" s="120" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="64"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" s="64"/>
+      <c r="V8" s="121"/>
+    </row>
+    <row r="9" spans="2:22">
+      <c r="B9" s="2"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="6"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="93"/>
+      <c r="Q9" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="R9" s="54"/>
+      <c r="S9" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" s="54"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="55"/>
+    </row>
+    <row r="10" spans="2:22" ht="16" thickBot="1">
+      <c r="B10" s="2"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="6"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="92"/>
+      <c r="N10" s="92"/>
+      <c r="O10" s="93"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="55"/>
+    </row>
+    <row r="11" spans="2:22">
+      <c r="B11" s="2"/>
+      <c r="C11" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="75"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="93"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="55"/>
+    </row>
+    <row r="12" spans="2:22">
+      <c r="B12" s="2"/>
+      <c r="C12" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="75"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="93"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="54"/>
+      <c r="U12" s="54"/>
+      <c r="V12" s="55"/>
+    </row>
+    <row r="13" spans="2:22">
+      <c r="B13" s="2"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="69"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="92"/>
+      <c r="O13" s="93"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
+      <c r="V13" s="55"/>
+    </row>
+    <row r="14" spans="2:22">
+      <c r="B14" s="2"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
+      <c r="O14" s="93"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="54"/>
+      <c r="V14" s="55"/>
+    </row>
+    <row r="15" spans="2:22">
+      <c r="B15" s="2">
+        <v>7</v>
+      </c>
+      <c r="C15" s="111"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="93"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="54"/>
+      <c r="U15" s="54"/>
+      <c r="V15" s="55"/>
+    </row>
+    <row r="16" spans="2:22" ht="16" thickBot="1">
+      <c r="B16" s="2"/>
+      <c r="C16" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="74"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="93"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="54"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="55"/>
+    </row>
+    <row r="17" spans="2:22">
+      <c r="B17" s="2"/>
+      <c r="C17" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="85"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="93"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="54"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="55"/>
+    </row>
+    <row r="18" spans="2:22">
+      <c r="B18" s="2"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="69"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="92"/>
+      <c r="M18" s="92"/>
+      <c r="N18" s="92"/>
+      <c r="O18" s="93"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="55"/>
+    </row>
+    <row r="19" spans="2:22">
+      <c r="B19" s="2"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="93"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="56"/>
+      <c r="T19" s="54"/>
+      <c r="U19" s="54"/>
+      <c r="V19" s="55"/>
+    </row>
+    <row r="20" spans="2:22">
+      <c r="B20" s="2"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="92"/>
+      <c r="N20" s="92"/>
+      <c r="O20" s="93"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="54"/>
+      <c r="U20" s="54"/>
+      <c r="V20" s="55"/>
+    </row>
+    <row r="21" spans="2:22">
+      <c r="B21" s="2"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="92"/>
+      <c r="M21" s="92"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="93"/>
+      <c r="Q21" s="53"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="54"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="55"/>
+    </row>
+    <row r="22" spans="2:22">
+      <c r="B22" s="2"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="93"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="56"/>
+      <c r="T22" s="54"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="55"/>
+    </row>
+    <row r="23" spans="2:22">
+      <c r="B23" s="2"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="92"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="92"/>
+      <c r="O23" s="93"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="55"/>
+    </row>
+    <row r="24" spans="2:22">
+      <c r="B24" s="2"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="92"/>
+      <c r="M24" s="92"/>
+      <c r="N24" s="92"/>
+      <c r="O24" s="93"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="56"/>
+      <c r="T24" s="54"/>
+      <c r="U24" s="54"/>
+      <c r="V24" s="55"/>
+    </row>
+    <row r="25" spans="2:22">
+      <c r="B25" s="2"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="92"/>
+      <c r="N25" s="92"/>
+      <c r="O25" s="93"/>
+      <c r="Q25" s="53"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="54"/>
+      <c r="U25" s="54"/>
+      <c r="V25" s="55"/>
+    </row>
+    <row r="26" spans="2:22">
+      <c r="B26" s="2"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
+      <c r="M26" s="92"/>
+      <c r="N26" s="92"/>
+      <c r="O26" s="93"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="56"/>
+      <c r="T26" s="54"/>
+      <c r="U26" s="54"/>
+      <c r="V26" s="55"/>
+    </row>
+    <row r="27" spans="2:22">
+      <c r="B27" s="2"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="31"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="92"/>
+      <c r="L27" s="92"/>
+      <c r="M27" s="92"/>
+      <c r="N27" s="92"/>
+      <c r="O27" s="93"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="54"/>
+      <c r="U27" s="54"/>
+      <c r="V27" s="55"/>
+    </row>
+    <row r="28" spans="2:22">
+      <c r="B28" s="2"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="31"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="92"/>
+      <c r="L28" s="92"/>
+      <c r="M28" s="92"/>
+      <c r="N28" s="92"/>
+      <c r="O28" s="93"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="54"/>
+      <c r="U28" s="54"/>
+      <c r="V28" s="55"/>
+    </row>
+    <row r="29" spans="2:22">
+      <c r="B29" s="2"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="92"/>
+      <c r="M29" s="92"/>
+      <c r="N29" s="92"/>
+      <c r="O29" s="93"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="54"/>
+      <c r="U29" s="54"/>
+      <c r="V29" s="55"/>
+    </row>
+    <row r="30" spans="2:22">
+      <c r="B30" s="2"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="92"/>
+      <c r="L30" s="92"/>
+      <c r="M30" s="92"/>
+      <c r="N30" s="92"/>
+      <c r="O30" s="93"/>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="56"/>
+      <c r="T30" s="54"/>
+      <c r="U30" s="54"/>
+      <c r="V30" s="55"/>
+    </row>
+    <row r="31" spans="2:22">
+      <c r="B31" s="2"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="92"/>
+      <c r="M31" s="92"/>
+      <c r="N31" s="92"/>
+      <c r="O31" s="93"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="54"/>
+      <c r="U31" s="54"/>
+      <c r="V31" s="55"/>
+    </row>
+    <row r="32" spans="2:22">
+      <c r="B32" s="2"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="92"/>
+      <c r="L32" s="92"/>
+      <c r="M32" s="92"/>
+      <c r="N32" s="92"/>
+      <c r="O32" s="93"/>
+      <c r="Q32" s="53"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="56"/>
+      <c r="T32" s="54"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="55"/>
+    </row>
+    <row r="33" spans="2:22">
+      <c r="B33" s="2">
+        <v>8</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="92"/>
+      <c r="L33" s="92"/>
+      <c r="M33" s="92"/>
+      <c r="N33" s="92"/>
+      <c r="O33" s="93"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="54"/>
+      <c r="U33" s="54"/>
+      <c r="V33" s="55"/>
+    </row>
+    <row r="34" spans="2:22" ht="16" thickBot="1">
+      <c r="B34" s="2"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
+      <c r="J34" s="94"/>
+      <c r="K34" s="95"/>
+      <c r="L34" s="95"/>
+      <c r="M34" s="95"/>
+      <c r="N34" s="95"/>
+      <c r="O34" s="96"/>
+      <c r="Q34" s="101"/>
+      <c r="R34" s="102"/>
+      <c r="S34" s="103"/>
+      <c r="T34" s="102"/>
+      <c r="U34" s="102"/>
+      <c r="V34" s="104"/>
+    </row>
+    <row r="35" spans="2:22" ht="16" thickBot="1">
+      <c r="B35" s="2"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
+      <c r="J35" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="20"/>
+      <c r="Q35" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="20"/>
+    </row>
+    <row r="36" spans="2:22">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:22">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="2:22">
+      <c r="B38" s="2">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D13:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="K4:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C18:H34"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="R4:V6"/>
+    <mergeCell ref="Q35:V35"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="Q7:V7"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:H8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Enhanemcents for new 3-panel dupfinder
</commit_message>
<xml_diff>
--- a/docs/find_dupicates-layout.xlsx
+++ b/docs/find_dupicates-layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Select Folders</t>
   </si>
@@ -91,9 +91,6 @@
     <t>o  Find Duplicates</t>
   </si>
   <si>
-    <t>(Power Options)</t>
-  </si>
-  <si>
     <t>Compare View</t>
   </si>
   <si>
@@ -122,6 +119,15 @@
   </si>
   <si>
     <t>+ Size x 1</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>(Extra Options)</t>
+  </si>
+  <si>
+    <t>You may type in folder name directly to add for exclusion(+)</t>
   </si>
 </sst>
 </file>
@@ -985,7 +991,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -1050,6 +1056,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1063,9 +1073,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -1088,201 +1095,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="37" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="56" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1303,18 +1127,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1"/>
@@ -1322,33 +1134,171 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="58" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="56" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="49" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1361,17 +1311,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="43" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -1402,6 +1406,8 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -1432,6 +1438,8 @@
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
@@ -1811,26 +1819,26 @@
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="49" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="50"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="4"/>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="22" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="10">
+      <c r="N3" s="59"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1838,31 +1846,31 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
       <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="64">
         <v>2</v>
       </c>
     </row>
@@ -1870,45 +1878,45 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="9" t="s">
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="17" t="s">
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="21"/>
+      <c r="P5" s="64"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
-      <c r="J6" s="12" t="s">
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="48"/>
+      <c r="J6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="K6" s="43"/>
@@ -1916,467 +1924,468 @@
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
       <c r="O6" s="45"/>
-      <c r="P6" s="21"/>
+      <c r="P6" s="64"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
-      <c r="J7" s="12" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48"/>
+      <c r="J7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="21"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="64"/>
     </row>
     <row r="8" spans="1:16" ht="16" thickBot="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
-      <c r="J8" s="13" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="54"/>
+      <c r="J8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="21"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="64"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="J9" s="27" t="s">
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="57"/>
+      <c r="J9" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="10">
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="10">
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="48"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="10"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="10"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="10"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="10"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="10"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="10"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="9"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="2"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="10"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="9"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="10"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="2"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="10"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="2"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="10"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="9"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="2"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="10"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="9"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="2"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="10"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="48"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="9"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="2"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="10"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="2"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="10"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="48"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="9"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="2"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="10"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="9"/>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="2"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="10"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="54"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="9"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="2">
         <v>8</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-      <c r="J27" s="36" t="s">
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="57"/>
+      <c r="J27" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="10">
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="57"/>
+      <c r="P27" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="2"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="10">
+      <c r="B28" s="46"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="2"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="10"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="9"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="2"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="10"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="9"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="2"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="10"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="54"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="9"/>
     </row>
     <row r="32" spans="1:16" ht="16" thickBot="1">
       <c r="A32" s="2">
         <v>9</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="10">
+      <c r="B32" s="61"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="9">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="K6:O8"/>
-    <mergeCell ref="J10:O26"/>
-    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="B28:G31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="J28:O31"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="J3:L3"/>
@@ -2384,14 +2393,13 @@
     <mergeCell ref="P4:P8"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="J9:O9"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="K6:O8"/>
+    <mergeCell ref="J10:O26"/>
+    <mergeCell ref="J27:O27"/>
     <mergeCell ref="C6:G8"/>
     <mergeCell ref="B10:G26"/>
-    <mergeCell ref="B28:G31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2408,7 +2416,7 @@
   <dimension ref="B2:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="D4" sqref="D4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2439,784 +2447,788 @@
       </c>
     </row>
     <row r="3" spans="2:22">
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="81" t="s">
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="82"/>
-      <c r="H3" s="83"/>
-      <c r="J3" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="105" t="s">
+      <c r="G3" s="88"/>
+      <c r="H3" s="89"/>
+      <c r="J3" s="39" t="s">
         <v>24</v>
+      </c>
+      <c r="K3" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="39" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:22">
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="51" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="112" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="114"/>
-      <c r="Q4" s="51" t="s">
+      <c r="K4" s="90" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="Q4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="112" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" s="113"/>
-      <c r="T4" s="113"/>
-      <c r="U4" s="113"/>
-      <c r="V4" s="114"/>
+      <c r="R4" s="90" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
     </row>
     <row r="5" spans="2:22">
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="106"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="107"/>
-      <c r="O5" s="115"/>
-      <c r="Q5" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="106"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="115"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="121"/>
+      <c r="J5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="93"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="95"/>
+      <c r="Q5" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" s="93"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="95"/>
     </row>
     <row r="6" spans="2:22" ht="16" thickBot="1">
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-      <c r="J6" s="51" t="s">
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="J6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="116"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="118"/>
-      <c r="Q6" s="51" t="s">
+      <c r="K6" s="96"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="98"/>
+      <c r="Q6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="116"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="117"/>
-      <c r="U6" s="117"/>
-      <c r="V6" s="118"/>
+      <c r="R6" s="96"/>
+      <c r="S6" s="97"/>
+      <c r="T6" s="97"/>
+      <c r="U6" s="97"/>
+      <c r="V6" s="98"/>
     </row>
     <row r="7" spans="2:22">
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="J7" s="108" t="s">
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="48"/>
+      <c r="J7" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="109"/>
-      <c r="Q7" s="98" t="s">
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="101"/>
+      <c r="Q7" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="99"/>
-      <c r="V7" s="100"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+      <c r="V7" s="117"/>
     </row>
     <row r="8" spans="2:22">
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="J8" s="119" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
-      <c r="O8" s="91"/>
-      <c r="Q8" s="120" t="s">
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
+      <c r="J8" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="29"/>
+      <c r="Q8" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="64"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="65" t="s">
+      <c r="R8" s="111"/>
+      <c r="S8" s="112"/>
+      <c r="T8" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="U8" s="64"/>
-      <c r="V8" s="121"/>
+      <c r="U8" s="111"/>
+      <c r="V8" s="114"/>
     </row>
     <row r="9" spans="2:22">
       <c r="B9" s="2"/>
-      <c r="C9" s="70"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="6"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="92" t="s">
+      <c r="J9" s="25"/>
+      <c r="K9" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="92"/>
-      <c r="N9" s="92"/>
-      <c r="O9" s="93"/>
-      <c r="Q9" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="R9" s="54"/>
-      <c r="S9" s="56" t="s">
+      <c r="L9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="55"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="31"/>
+      <c r="Q9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="19"/>
+      <c r="S9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="20"/>
     </row>
     <row r="10" spans="2:22" ht="16" thickBot="1">
       <c r="B10" s="2"/>
-      <c r="C10" s="70"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="6"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="92" t="s">
+      <c r="J10" s="25"/>
+      <c r="K10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="92"/>
-      <c r="N10" s="92"/>
-      <c r="O10" s="93"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="54"/>
-      <c r="U10" s="54"/>
-      <c r="V10" s="55"/>
+      <c r="L10" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="31"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="20"/>
     </row>
     <row r="11" spans="2:22">
       <c r="B11" s="2"/>
-      <c r="C11" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="97" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="75"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="93"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="54"/>
-      <c r="U11" s="54"/>
-      <c r="V11" s="55"/>
+      <c r="C11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="20"/>
     </row>
     <row r="12" spans="2:22">
       <c r="B12" s="2"/>
-      <c r="C12" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="57" t="s">
+      <c r="C12" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="75"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="92"/>
-      <c r="O12" s="93"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="54"/>
-      <c r="U12" s="54"/>
-      <c r="V12" s="55"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="121"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="20"/>
     </row>
     <row r="13" spans="2:22">
       <c r="B13" s="2"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="69"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="92"/>
-      <c r="L13" s="92"/>
-      <c r="M13" s="92"/>
-      <c r="N13" s="92"/>
-      <c r="O13" s="93"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="54"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="54"/>
-      <c r="U13" s="54"/>
-      <c r="V13" s="55"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="31"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="20"/>
     </row>
     <row r="14" spans="2:22">
       <c r="B14" s="2"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="92"/>
-      <c r="O14" s="93"/>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="54"/>
-      <c r="V14" s="55"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="48"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="20"/>
     </row>
     <row r="15" spans="2:22">
       <c r="B15" s="2">
         <v>7</v>
       </c>
-      <c r="C15" s="111"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
-      <c r="N15" s="92"/>
-      <c r="O15" s="93"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
-      <c r="V15" s="55"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="54"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="31"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="20"/>
     </row>
     <row r="16" spans="2:22" ht="16" thickBot="1">
       <c r="B16" s="2"/>
-      <c r="C16" s="71" t="s">
+      <c r="C16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="74"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
-      <c r="O16" s="93"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="54"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="54"/>
-      <c r="U16" s="54"/>
-      <c r="V16" s="55"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="20"/>
     </row>
     <row r="17" spans="2:22">
       <c r="B17" s="2"/>
-      <c r="C17" s="84" t="s">
+      <c r="C17" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="85"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="92"/>
-      <c r="L17" s="92"/>
-      <c r="M17" s="92"/>
-      <c r="N17" s="92"/>
-      <c r="O17" s="93"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="55"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="107"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="31"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="20"/>
     </row>
     <row r="18" spans="2:22">
       <c r="B18" s="2"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="69"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="92"/>
-      <c r="M18" s="92"/>
-      <c r="N18" s="92"/>
-      <c r="O18" s="93"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
+      <c r="C18" s="104"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="79"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="31"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="20"/>
     </row>
     <row r="19" spans="2:22">
       <c r="B19" s="2"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="92"/>
-      <c r="M19" s="92"/>
-      <c r="N19" s="92"/>
-      <c r="O19" s="93"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="54"/>
-      <c r="S19" s="56"/>
-      <c r="T19" s="54"/>
-      <c r="U19" s="54"/>
-      <c r="V19" s="55"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="20"/>
     </row>
     <row r="20" spans="2:22">
       <c r="B20" s="2"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="92"/>
-      <c r="M20" s="92"/>
-      <c r="N20" s="92"/>
-      <c r="O20" s="93"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="54"/>
-      <c r="U20" s="54"/>
-      <c r="V20" s="55"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="31"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="20"/>
     </row>
     <row r="21" spans="2:22">
       <c r="B21" s="2"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="31"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="92"/>
-      <c r="L21" s="92"/>
-      <c r="M21" s="92"/>
-      <c r="N21" s="92"/>
-      <c r="O21" s="93"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="54"/>
-      <c r="V21" s="55"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="20"/>
     </row>
     <row r="22" spans="2:22">
       <c r="B22" s="2"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="92"/>
-      <c r="L22" s="92"/>
-      <c r="M22" s="92"/>
-      <c r="N22" s="92"/>
-      <c r="O22" s="93"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="54"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="55"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="48"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="20"/>
     </row>
     <row r="23" spans="2:22">
       <c r="B23" s="2"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="92"/>
-      <c r="M23" s="92"/>
-      <c r="N23" s="92"/>
-      <c r="O23" s="93"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="55"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="48"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="20"/>
     </row>
     <row r="24" spans="2:22">
       <c r="B24" s="2"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="31"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="92"/>
-      <c r="N24" s="92"/>
-      <c r="O24" s="93"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="54"/>
-      <c r="U24" s="54"/>
-      <c r="V24" s="55"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="48"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="31"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="20"/>
     </row>
     <row r="25" spans="2:22">
       <c r="B25" s="2"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="93"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="56"/>
-      <c r="T25" s="54"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="55"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="48"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="31"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="20"/>
     </row>
     <row r="26" spans="2:22">
       <c r="B26" s="2"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="92"/>
-      <c r="M26" s="92"/>
-      <c r="N26" s="92"/>
-      <c r="O26" s="93"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="56"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="55"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="48"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="31"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="20"/>
     </row>
     <row r="27" spans="2:22">
       <c r="B27" s="2"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="92"/>
-      <c r="L27" s="92"/>
-      <c r="M27" s="92"/>
-      <c r="N27" s="92"/>
-      <c r="O27" s="93"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="54"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="54"/>
-      <c r="U27" s="54"/>
-      <c r="V27" s="55"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="48"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="31"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="20"/>
     </row>
     <row r="28" spans="2:22">
       <c r="B28" s="2"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="31"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="92"/>
-      <c r="L28" s="92"/>
-      <c r="M28" s="92"/>
-      <c r="N28" s="92"/>
-      <c r="O28" s="93"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="54"/>
-      <c r="U28" s="54"/>
-      <c r="V28" s="55"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="48"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="31"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="20"/>
     </row>
     <row r="29" spans="2:22">
       <c r="B29" s="2"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="92"/>
-      <c r="L29" s="92"/>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92"/>
-      <c r="O29" s="93"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="54"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="54"/>
-      <c r="U29" s="54"/>
-      <c r="V29" s="55"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="48"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="31"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="20"/>
     </row>
     <row r="30" spans="2:22">
       <c r="B30" s="2"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="31"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="92"/>
-      <c r="L30" s="92"/>
-      <c r="M30" s="92"/>
-      <c r="N30" s="92"/>
-      <c r="O30" s="93"/>
-      <c r="Q30" s="53"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="54"/>
-      <c r="U30" s="54"/>
-      <c r="V30" s="55"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="31"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="20"/>
     </row>
     <row r="31" spans="2:22">
       <c r="B31" s="2"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="92"/>
-      <c r="L31" s="92"/>
-      <c r="M31" s="92"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="93"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="54"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="54"/>
-      <c r="U31" s="54"/>
-      <c r="V31" s="55"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="48"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="31"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="20"/>
     </row>
     <row r="32" spans="2:22">
       <c r="B32" s="2"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="31"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="92"/>
-      <c r="L32" s="92"/>
-      <c r="M32" s="92"/>
-      <c r="N32" s="92"/>
-      <c r="O32" s="93"/>
-      <c r="Q32" s="53"/>
-      <c r="R32" s="54"/>
-      <c r="S32" s="56"/>
-      <c r="T32" s="54"/>
-      <c r="U32" s="54"/>
-      <c r="V32" s="55"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="48"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="31"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="20"/>
     </row>
     <row r="33" spans="2:22">
       <c r="B33" s="2">
         <v>8</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="92"/>
-      <c r="L33" s="92"/>
-      <c r="M33" s="92"/>
-      <c r="N33" s="92"/>
-      <c r="O33" s="93"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="54"/>
-      <c r="S33" s="56"/>
-      <c r="T33" s="54"/>
-      <c r="U33" s="54"/>
-      <c r="V33" s="55"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="48"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="31"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="20"/>
     </row>
     <row r="34" spans="2:22" ht="16" thickBot="1">
       <c r="B34" s="2"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="33"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="95"/>
-      <c r="L34" s="95"/>
-      <c r="M34" s="95"/>
-      <c r="N34" s="95"/>
-      <c r="O34" s="96"/>
-      <c r="Q34" s="101"/>
-      <c r="R34" s="102"/>
-      <c r="S34" s="103"/>
-      <c r="T34" s="102"/>
-      <c r="U34" s="102"/>
-      <c r="V34" s="104"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="54"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="37"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
+      <c r="V34" s="38"/>
     </row>
     <row r="35" spans="2:22" ht="16" thickBot="1">
       <c r="B35" s="2"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="20"/>
-      <c r="J35" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="20"/>
-      <c r="Q35" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="20"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="63"/>
+      <c r="J35" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="63"/>
+      <c r="Q35" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="R35" s="62"/>
+      <c r="S35" s="62"/>
+      <c r="T35" s="62"/>
+      <c r="U35" s="62"/>
+      <c r="V35" s="63"/>
     </row>
     <row r="36" spans="2:22">
       <c r="B36" s="2"/>
@@ -3231,11 +3243,13 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D13:H15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="R4:V6"/>
+    <mergeCell ref="Q35:V35"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="Q7:V7"/>
     <mergeCell ref="J35:O35"/>
     <mergeCell ref="K4:O6"/>
     <mergeCell ref="J7:O7"/>
@@ -3243,15 +3257,13 @@
     <mergeCell ref="C18:H34"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="C35:H35"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="R4:V6"/>
-    <mergeCell ref="Q35:V35"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="Q7:V7"/>
     <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
     <mergeCell ref="D6:H8"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D13:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>